<commit_message>
Update detectors comments, and ground truth; remove dataset artifacts
</commit_message>
<xml_diff>
--- a/Ground Truth/test_ground_truth.xlsx
+++ b/Ground Truth/test_ground_truth.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29725"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Yasin\Desktop\New folder\master thesis\Shot-Boundary-Detection\Ground Truth\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Yasin\Desktop\Publication\Shot-Boundary-Detection\Ground Truth\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7679B799-402B-4DBC-A1E3-FE1145AA0D59}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC395755-8579-4EA0-91AA-ED7A4C168B85}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-19320" yWindow="-4785" windowWidth="19440" windowHeight="14880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,10 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
-  <si>
-    <t>video</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="44">
   <si>
     <t>ground truth</t>
   </si>
@@ -63,21 +60,6 @@
     <t>1009-1028,1555-1574</t>
   </si>
   <si>
-    <t>test_bundesliga</t>
-  </si>
-  <si>
-    <t>test_epl</t>
-  </si>
-  <si>
-    <t>test_italy</t>
-  </si>
-  <si>
-    <t>test_UEFA</t>
-  </si>
-  <si>
-    <t>test_france</t>
-  </si>
-  <si>
     <t>7</t>
   </si>
   <si>
@@ -115,13 +97,73 @@
   </si>
   <si>
     <t>0,348,409,534,571,616,682,711,813,870,918,1020,1029,1284,1411,1566,1575,1804,1956</t>
+  </si>
+  <si>
+    <t>2015-02-21 - 17-30 Paderborn 0 - 6 Bayern Munich</t>
+  </si>
+  <si>
+    <t>17:55</t>
+  </si>
+  <si>
+    <t>2015-02-21 - 18-00 Crystal Palace 1 - 2 Arsenal</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>45:08</t>
+  </si>
+  <si>
+    <t>2015-04-05 - 22-00 Marseille 2 - 3 Paris SG</t>
+  </si>
+  <si>
+    <t>05:48</t>
+  </si>
+  <si>
+    <t>2016-08-21 - 21-45 Pescara 2 - 2 Napoli</t>
+  </si>
+  <si>
+    <t>34:54</t>
+  </si>
+  <si>
+    <t>2017-03-08 - 22-45 Barcelona 6 - 1 Paris SG</t>
+  </si>
+  <si>
+    <t>39:24</t>
+  </si>
+  <si>
+    <t>Match</t>
+  </si>
+  <si>
+    <t>Game half</t>
+  </si>
+  <si>
+    <t>Game time (min:sec)</t>
+  </si>
+  <si>
+    <t>League</t>
+  </si>
+  <si>
+    <t>bundesliga</t>
+  </si>
+  <si>
+    <t>epl</t>
+  </si>
+  <si>
+    <t>france</t>
+  </si>
+  <si>
+    <t>italy</t>
+  </si>
+  <si>
+    <t>UEFA</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -144,6 +186,13 @@
     <font>
       <b/>
       <sz val="14"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -171,15 +220,17 @@
   </cellStyleXfs>
   <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -461,134 +512,183 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E9"/>
+  <dimension ref="A1:H9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="29.44140625" style="2" customWidth="1"/>
-    <col min="2" max="2" width="63.33203125" style="2" customWidth="1"/>
-    <col min="3" max="3" width="17.88671875" style="2" customWidth="1"/>
-    <col min="4" max="4" width="26.21875" style="2" customWidth="1"/>
-    <col min="5" max="5" width="20.6640625" style="2" customWidth="1"/>
-    <col min="6" max="6" width="16.21875" style="2" customWidth="1"/>
-    <col min="7" max="16384" width="8.88671875" style="2"/>
+    <col min="1" max="1" width="35.21875" style="4" customWidth="1"/>
+    <col min="2" max="3" width="8.88671875" style="4"/>
+    <col min="4" max="4" width="29.44140625" style="4" customWidth="1"/>
+    <col min="5" max="5" width="63.33203125" style="4" customWidth="1"/>
+    <col min="6" max="6" width="17.88671875" style="4" customWidth="1"/>
+    <col min="7" max="7" width="26.21875" style="4" customWidth="1"/>
+    <col min="8" max="8" width="20.6640625" style="4" customWidth="1"/>
+    <col min="9" max="9" width="16.21875" style="4" customWidth="1"/>
+    <col min="10" max="16384" width="8.88671875" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="18" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:8" s="4" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="F1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="G1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="H1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="4" t="s">
+    </row>
+    <row r="2" spans="1:8" s="4" customFormat="1" ht="36" x14ac:dyDescent="0.3">
+      <c r="A2" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="H2" s="3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="36" x14ac:dyDescent="0.35">
-      <c r="A2" s="1" t="s">
+    <row r="3" spans="1:8" s="4" customFormat="1" ht="36" x14ac:dyDescent="0.3">
+      <c r="A3" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="F3" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="C2" s="1" t="s">
+      <c r="G3" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="H3" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" s="4" customFormat="1" ht="36" x14ac:dyDescent="0.3">
+      <c r="A4" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="G4" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="H4" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="E2" s="1" t="s">
-        <v>5</v>
-      </c>
     </row>
-    <row r="3" spans="1:5" ht="36" x14ac:dyDescent="0.35">
-      <c r="A3" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="E3" s="1" t="s">
+    <row r="5" spans="1:8" s="4" customFormat="1" ht="54" x14ac:dyDescent="0.3">
+      <c r="A5" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="E5" s="3" t="s">
         <v>22</v>
       </c>
+      <c r="F5" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="G5" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="H5" s="3" t="s">
+        <v>8</v>
+      </c>
     </row>
-    <row r="4" spans="1:5" ht="36" x14ac:dyDescent="0.35">
-      <c r="A4" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="B4" s="1" t="s">
+    <row r="6" spans="1:8" s="4" customFormat="1" ht="36" x14ac:dyDescent="0.3">
+      <c r="A6" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B6" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="C4" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="D4" s="1" t="s">
+      <c r="C6" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="E6" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="E4" s="1" t="s">
-        <v>7</v>
+      <c r="F6" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="G6" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="H6" s="3" t="s">
+        <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="54" x14ac:dyDescent="0.35">
-      <c r="A5" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" ht="36" x14ac:dyDescent="0.35">
-      <c r="A6" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A7" s="3"/>
-      <c r="C7" s="3"/>
-      <c r="D7" s="3"/>
-      <c r="E7" s="3"/>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B9" s="3"/>
-    </row>
+    <row r="7" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="9" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>